<commit_message>
added excel data export
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -8,6 +8,26 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet11" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet12" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet13" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet15" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet16" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet17" sheetId="18" r:id="rId18"/>
+    <sheet name="Sheet18" sheetId="19" r:id="rId19"/>
+    <sheet name="Sheet19" sheetId="20" r:id="rId20"/>
+    <sheet name="Sheet20" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>login</t>
   </si>
@@ -40,13 +60,313 @@
   </si>
   <si>
     <t>failedLogin</t>
+  </si>
+  <si>
+    <t>Відповідач(боржник)</t>
+  </si>
+  <si>
+    <t>Відпоборжник В.А.</t>
+  </si>
+  <si>
+    <t>Відповідач</t>
+  </si>
+  <si>
+    <t>ВідпоДоПрокуратури А.е.</t>
+  </si>
+  <si>
+    <t>Дата реєстрації</t>
+  </si>
+  <si>
+    <t>Статті КК України за ознаками яких розпочато кримінальне провадження</t>
+  </si>
+  <si>
+    <t>Фабула</t>
+  </si>
+  <si>
+    <t>04.05.2017</t>
+  </si>
+  <si>
+    <t>Фабула 89758973548 :?%№!  -- Pvbcshgbcvghsacvgh</t>
+  </si>
+  <si>
+    <t>Стаття 56342423422 пункт 45 Гавсміот</t>
+  </si>
+  <si>
+    <t>Кваліфікація правопорушення/злочину</t>
+  </si>
+  <si>
+    <t>Дата  початку досудового розслідування:</t>
+  </si>
+  <si>
+    <t>Зміст(фабула)</t>
+  </si>
+  <si>
+    <t>Кваліфікаці897786675</t>
+  </si>
+  <si>
+    <t>11.11.2016</t>
+  </si>
+  <si>
+    <t>Зміст 43252Pvbcshgbcvghsacvgh</t>
+  </si>
+  <si>
+    <t>ПІБ підозрюваного / обвинуваченого</t>
+  </si>
+  <si>
+    <t>Підстави для оскарження</t>
+  </si>
+  <si>
+    <t>Кваліфііфвфввфввф32</t>
+  </si>
+  <si>
+    <t>Підозрюваний1 П.ОГ.</t>
+  </si>
+  <si>
+    <t>Кваііфіфф354354</t>
+  </si>
+  <si>
+    <t>Підозрюваниві Р.О.</t>
+  </si>
+  <si>
+    <t>віаіваі4325356авпа535</t>
+  </si>
+  <si>
+    <t>3443243аавіаві</t>
+  </si>
+  <si>
+    <t>Прізвище</t>
+  </si>
+  <si>
+    <t>Ім'я</t>
+  </si>
+  <si>
+    <t>Дата народження</t>
+  </si>
+  <si>
+    <t>Кваліфікація</t>
+  </si>
+  <si>
+    <t>23.02.2017</t>
+  </si>
+  <si>
+    <t>Прімтомва</t>
+  </si>
+  <si>
+    <t>Ввіоіфлар</t>
+  </si>
+  <si>
+    <t>11.11.1967</t>
+  </si>
+  <si>
+    <t>23.02.2016</t>
+  </si>
+  <si>
+    <t>аіавм</t>
+  </si>
+  <si>
+    <t>ава</t>
+  </si>
+  <si>
+    <t>13.09.1968</t>
+  </si>
+  <si>
+    <t>Номер справи у суді</t>
+  </si>
+  <si>
+    <t>Дата прийняття остаточного рішення у КП стосовно особи</t>
+  </si>
+  <si>
+    <t>11.06.2014</t>
+  </si>
+  <si>
+    <t>Справа6876468326_оо</t>
+  </si>
+  <si>
+    <t>Дата прийняття рішення</t>
+  </si>
+  <si>
+    <t>17.07.2015</t>
+  </si>
+  <si>
+    <t>Дата рішення суду</t>
+  </si>
+  <si>
+    <t>21.01.2013</t>
+  </si>
+  <si>
+    <t>Дата початку досудового розслідування</t>
+  </si>
+  <si>
+    <t>Кваліфікація правопорушення</t>
+  </si>
+  <si>
+    <t>Дата надіслання до суду</t>
+  </si>
+  <si>
+    <t>Квіваів8532856934</t>
+  </si>
+  <si>
+    <t>08.12.2016</t>
+  </si>
+  <si>
+    <t>01.01.2017</t>
+  </si>
+  <si>
+    <t>08.12.2017</t>
+  </si>
+  <si>
+    <t>01.01.2018</t>
+  </si>
+  <si>
+    <t>Коротка фабула</t>
+  </si>
+  <si>
+    <t>іфвосвпіор6455656737</t>
+  </si>
+  <si>
+    <t>27.02.2017</t>
+  </si>
+  <si>
+    <t>10.10.2013</t>
+  </si>
+  <si>
+    <t>Кваліфітваи2358947564рпам</t>
+  </si>
+  <si>
+    <t>20.05.2012</t>
+  </si>
+  <si>
+    <t>01.03.2017</t>
+  </si>
+  <si>
+    <t>13.04.2013</t>
+  </si>
+  <si>
+    <t>31.03.2017</t>
+  </si>
+  <si>
+    <t>аоір**?%?:пррро09986523</t>
+  </si>
+  <si>
+    <t>Дата надходження</t>
+  </si>
+  <si>
+    <t>Стислий зміст</t>
+  </si>
+  <si>
+    <t>07.11.1955</t>
+  </si>
+  <si>
+    <t>Влоовмирівми9079687234123;%?*:*?(%?*:(?*</t>
+  </si>
+  <si>
+    <t>Дата проведення перевірки</t>
+  </si>
+  <si>
+    <t>14.11.2000</t>
+  </si>
+  <si>
+    <t>Посада</t>
+  </si>
+  <si>
+    <t>Посада бла-бла67675</t>
+  </si>
+  <si>
+    <t>Назва заявника</t>
+  </si>
+  <si>
+    <t>Дата надходження до прокуратури</t>
+  </si>
+  <si>
+    <t>07.06.2010</t>
+  </si>
+  <si>
+    <t>Заявник43897ав</t>
+  </si>
+  <si>
+    <t>ОИРпргспгвні784607*():%:?№;;%;</t>
+  </si>
+  <si>
+    <t>Дата виступу</t>
+  </si>
+  <si>
+    <t>Назва ЗМІ</t>
+  </si>
+  <si>
+    <t>Автор</t>
+  </si>
+  <si>
+    <t>Примітка</t>
+  </si>
+  <si>
+    <t>01.05.2017</t>
+  </si>
+  <si>
+    <t>Зміїшка?:%9078786</t>
+  </si>
+  <si>
+    <t>Авторрпрвш43</t>
+  </si>
+  <si>
+    <t>ОИРАпрвЕНАгне56342п*:*:%34%8</t>
+  </si>
+  <si>
+    <t>03.11.2015</t>
+  </si>
+  <si>
+    <t>мівм жбдло*::%;"?№:*(7гшппросмлі</t>
+  </si>
+  <si>
+    <t>Дата складання протоколу</t>
+  </si>
+  <si>
+    <t>Дата вчинення правопорушення</t>
+  </si>
+  <si>
+    <t>ПІБ правопорушника</t>
+  </si>
+  <si>
+    <t>Назва військової частини, установи</t>
+  </si>
+  <si>
+    <t>Дата первинного направлення до суду (для обліку у звіті)</t>
+  </si>
+  <si>
+    <t>Дата надходження рішення про повернення судом (для обліку у звіту)</t>
+  </si>
+  <si>
+    <t>Дата повторного направлення (для обліку у звіту)</t>
+  </si>
+  <si>
+    <t>Поле "Дата рішення</t>
+  </si>
+  <si>
+    <t>Дата надходження рішення суду(для обліку у звіті)</t>
+  </si>
+  <si>
+    <t>Дата початку утримання на гаупвахті</t>
+  </si>
+  <si>
+    <t>01.07.2016</t>
+  </si>
+  <si>
+    <t>Фабулашргммн*?*:?№?;?*69</t>
+  </si>
+  <si>
+    <t>Првіфол. ШР. ШР</t>
+  </si>
+  <si>
+    <t>військова09(?№;!"№%:757978е</t>
+  </si>
+  <si>
+    <t>Посадафіооаоірао</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,12 +375,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -72,7 +399,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,13 +407,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,40 +717,45 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -411,4 +763,884 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="13" width="11.85546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>